<commit_message>
🐞Fix(Repair the token resolution fail, the user login authentication return value optimization problem, other known bugs): 修复token解析失败，用户登录认证返回值优化问题、其他已知bug
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitpush\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EEF748-5AF6-4DA9-B112-88DE30055B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772391B1-252B-45D7-8BFF-106E2EF44E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="288">
   <si>
     <t>id</t>
   </si>
@@ -635,52 +635,34 @@
     <t>web_title</t>
   </si>
   <si>
-    <t>Kinit</t>
-  </si>
-  <si>
     <t>系统LOGO</t>
   </si>
   <si>
     <t>web_logo</t>
   </si>
   <si>
-    <t>/media/system/2023-01-16/16738638056c6b786e.png</t>
-  </si>
-  <si>
     <t>系统描述</t>
   </si>
   <si>
     <t>web_desc</t>
   </si>
   <si>
-    <t>Kinit 是一套开箱即用的中后台解决方案，可以作为新项目的启动模版。</t>
-  </si>
-  <si>
     <t>ICO图标</t>
   </si>
   <si>
     <t>web_ico</t>
   </si>
   <si>
-    <t>/media/system/2023-01-16/16738638074695e982.ico</t>
-  </si>
-  <si>
     <t>备案号</t>
   </si>
   <si>
     <t>web_icp_number</t>
   </si>
   <si>
-    <t>豫ICP备19033601号-1</t>
-  </si>
-  <si>
     <t>版权信息</t>
   </si>
   <si>
     <t>web_copyright</t>
-  </si>
-  <si>
-    <t>Copyright ©2022-present K</t>
   </si>
   <si>
     <t>百度统计代码</t>
@@ -840,9 +822,6 @@
     <t>wx_server_email</t>
   </si>
   <si>
-    <t>2445667550@qq.com</t>
-  </si>
-  <si>
     <t>服务热线</t>
   </si>
   <si>
@@ -853,9 +832,6 @@
   </si>
   <si>
     <t>wx_server_site</t>
-  </si>
-  <si>
-    <t>http://kinit.ktianc.top</t>
   </si>
   <si>
     <t>AppID</t>
@@ -918,6 +894,102 @@
   </si>
   <si>
     <t>$2b$12$Ce7eSUKIIl8DMKeDyNHyr.Dp4aesQCM70RePigRVEny1Eql31R0Cq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>管理员</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://fastapi.tiangolo.com/img/icon-white.svg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>akura_k</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Sakura_k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是一套开箱即用的中后台解决方案，可以作为新项目的启动模版。</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b67fa252ad1e94f6e9fe515d5dcf37c</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ry@beidoucom.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>13206269804</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@163.com</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>em</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ail</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ry@beidoucom.com</t>
+  </si>
+  <si>
+    <t>$2b$12$1j53PS8lNyAdF4xv24DCx.l4FxHPe5OULqKv90yRDVEPi1lmLsxuG</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -928,7 +1000,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -958,6 +1030,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -982,13 +1063,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1267,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3327,10 +3428,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3338,111 +3439,176 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="7" max="7" width="72.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.140625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="Q1" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
         <v>44784.845185185201</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="10">
         <v>44888.896111111098</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
+      <c r="N2" s="10"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>45061.728391203702</v>
+      </c>
+      <c r="C3" s="11">
+        <v>45061.730069444442</v>
+      </c>
+      <c r="D3" s="8">
+        <v>13206269804</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="11">
+        <v>45061.729930555557</v>
+      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://fastapi.管理员.com/img/icon-white.svg" xr:uid="{123EAE1A-000B-476D-8B77-383D7C062274}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{7A742420-628F-4D78-8429-5535AE30F689}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4393,19 +4559,19 @@
         <v>44971.953680555598</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -4424,8 +4590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4433,7 +4599,7 @@
     <col min="2" max="3" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="98" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4488,8 +4654,8 @@
       <c r="F2" t="s">
         <v>191</v>
       </c>
-      <c r="G2" t="s">
-        <v>192</v>
+      <c r="G2" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -4512,13 +4678,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" t="s">
         <v>193</v>
-      </c>
-      <c r="F3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" t="s">
-        <v>195</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -4541,13 +4704,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -4570,13 +4733,10 @@
         <v>44942.757025462997</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -4599,13 +4759,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -4628,13 +4785,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -4657,13 +4811,13 @@
         <v>44887.691469907397</v>
       </c>
       <c r="E8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F8" t="s">
         <v>169</v>
       </c>
       <c r="H8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -4686,13 +4840,13 @@
         <v>44965.452013888898</v>
       </c>
       <c r="E9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
         <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -4721,7 +4875,7 @@
         <v>175</v>
       </c>
       <c r="G10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -4744,10 +4898,10 @@
         <v>44873.394305555601</v>
       </c>
       <c r="E11" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -4770,10 +4924,10 @@
         <v>44873.394861111097</v>
       </c>
       <c r="E12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -4796,13 +4950,13 @@
         <v>44873.397835648102</v>
       </c>
       <c r="E13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="I13">
         <v>6</v>
@@ -4825,13 +4979,13 @@
         <v>44873.404872685198</v>
       </c>
       <c r="E14" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H14" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -4854,13 +5008,13 @@
         <v>44873.948194444398</v>
       </c>
       <c r="E15" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F15" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G15" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -4883,13 +5037,13 @@
         <v>44873.948611111096</v>
       </c>
       <c r="E16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G16" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I16">
         <v>6</v>
@@ -4912,13 +5066,13 @@
         <v>44880.940173611103</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -4941,13 +5095,13 @@
         <v>44880.941412036998</v>
       </c>
       <c r="E18" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F18" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H18" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -4970,13 +5124,16 @@
         <v>44882.8044212963</v>
       </c>
       <c r="E19" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F19" t="s">
-        <v>236</v>
+        <v>230</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="H19" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I19">
         <v>8</v>
@@ -4999,16 +5156,16 @@
         <v>44882.805381944403</v>
       </c>
       <c r="E20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F20" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H20" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I20">
         <v>8</v>
@@ -5031,16 +5188,16 @@
         <v>44882.805740740703</v>
       </c>
       <c r="E21" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G21" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H21" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I21">
         <v>8</v>
@@ -5063,16 +5220,16 @@
         <v>44882.814594907402</v>
       </c>
       <c r="E22" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F22" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G22" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H22" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I22">
         <v>8</v>
@@ -5095,16 +5252,16 @@
         <v>44882.815324074101</v>
       </c>
       <c r="E23" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F23" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G23" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="H23" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I23">
         <v>8</v>
@@ -5127,16 +5284,16 @@
         <v>44882.816689814797</v>
       </c>
       <c r="E24" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G24" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H24" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I24">
         <v>8</v>
@@ -5159,13 +5316,13 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E25" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>259</v>
-      </c>
-      <c r="G25" t="s">
-        <v>260</v>
+        <v>253</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="I25">
         <v>9</v>
@@ -5188,10 +5345,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E26" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F26" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I26">
         <v>9</v>
@@ -5214,13 +5371,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E27" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F27" t="s">
-        <v>264</v>
-      </c>
-      <c r="G27" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="I27">
         <v>9</v>
@@ -5243,10 +5397,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E28" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="F28" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="I28">
         <v>9</v>
@@ -5269,10 +5423,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E29" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="F29" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="I29">
         <v>9</v>
@@ -5295,12 +5449,14 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="F30" t="s">
-        <v>275</v>
-      </c>
-      <c r="G30" s="4"/>
+        <v>267</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>284</v>
+      </c>
       <c r="I30">
         <v>10</v>
       </c>
@@ -5322,12 +5478,12 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F31" t="s">
-        <v>277</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>269</v>
+      </c>
+      <c r="G31" s="7"/>
       <c r="I31">
         <v>10</v>
       </c>
@@ -5349,13 +5505,13 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="F32" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="I32">
         <v>10</v>
@@ -5378,10 +5534,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F33" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G33" s="5">
         <v>25</v>
@@ -5398,6 +5554,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G25" r:id="rId1" xr:uid="{AB2F913A-073D-428C-A298-E0563D2AAD28}"/>
+    <hyperlink ref="G30" r:id="rId2" xr:uid="{AB4E9E47-7019-4F3A-9F9B-172570F9F010}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
🎈perf(Initial data update && Version number update ): 初始数据更新&&版本号更新
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitpush\Sakura_K\scripts\initialize\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\ktianc\project\kinit\kinit-api\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772391B1-252B-45D7-8BFF-106E2EF44E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B17DA4-D279-42B3-96AF-423A27C976FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-870" yWindow="4575" windowWidth="35895" windowHeight="15345" tabRatio="887" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="294">
   <si>
     <t>id</t>
   </si>
@@ -209,15 +209,6 @@
     <t>字典详情</t>
   </si>
   <si>
-    <t>views/Home/Home</t>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>个人主页</t>
-  </si>
-  <si>
     <t>record</t>
   </si>
   <si>
@@ -380,6 +371,21 @@
     <t>空气质量</t>
   </si>
   <si>
+    <t>views/vadmin/system/task/index</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>定时任务</t>
+  </si>
+  <si>
+    <t>views/vadmin/system/record/task/index</t>
+  </si>
+  <si>
+    <t>调度日志</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -425,10 +431,16 @@
     <t>last_login</t>
   </si>
   <si>
+    <t>is_staff</t>
+  </si>
+  <si>
     <t>15020221010</t>
   </si>
   <si>
     <t>kinit</t>
+  </si>
+  <si>
+    <t>$2b$12$Ce7eSUKIIl8DMKeDyNHyr.Dp4aesQCM70RePigRVEny1Eql31R0Cq</t>
   </si>
   <si>
     <t>127.0.0.1</t>
@@ -503,6 +515,15 @@
     <t>sys_vadmin_platform</t>
   </si>
   <si>
+    <t>定时任务执行策略</t>
+  </si>
+  <si>
+    <t>vadmin_system_task_exec_strategy</t>
+  </si>
+  <si>
+    <t>与定时任务中有约定，请勿随意更改</t>
+  </si>
+  <si>
     <t>is_default</t>
   </si>
   <si>
@@ -545,6 +566,24 @@
     <t>微信一键登录</t>
   </si>
   <si>
+    <t>时间间隔(interval)</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>Cron 表达式</t>
+  </si>
+  <si>
+    <t>cron</t>
+  </si>
+  <si>
+    <t>指定日期时间(date)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>tab_label</t>
   </si>
   <si>
@@ -617,6 +656,12 @@
     <t>wx_server</t>
   </si>
   <si>
+    <t>邮箱配置</t>
+  </si>
+  <si>
+    <t>web_email</t>
+  </si>
+  <si>
     <t>config_label</t>
   </si>
   <si>
@@ -635,6 +680,9 @@
     <t>web_title</t>
   </si>
   <si>
+    <t>Kinit</t>
+  </si>
+  <si>
     <t>系统LOGO</t>
   </si>
   <si>
@@ -647,6 +695,9 @@
     <t>web_desc</t>
   </si>
   <si>
+    <t>Kinit 是一套开箱即用的中后台解决方案，可以作为新项目的启动模版。</t>
+  </si>
+  <si>
     <t>ICO图标</t>
   </si>
   <si>
@@ -659,10 +710,16 @@
     <t>web_icp_number</t>
   </si>
   <si>
+    <t>豫ICP备19033601号-1</t>
+  </si>
+  <si>
     <t>版权信息</t>
   </si>
   <si>
     <t>web_copyright</t>
+  </si>
+  <si>
+    <t>Copyright ©2022-present K</t>
   </si>
   <si>
     <t>百度统计代码</t>
@@ -822,6 +879,9 @@
     <t>wx_server_email</t>
   </si>
   <si>
+    <t>2445667550@qq.com</t>
+  </si>
+  <si>
     <t>服务热线</t>
   </si>
   <si>
@@ -834,6 +894,9 @@
     <t>wx_server_site</t>
   </si>
   <si>
+    <t>http://kinit.ktianc.top</t>
+  </si>
+  <si>
     <t>AppID</t>
   </si>
   <si>
@@ -846,22 +909,6 @@
     <t>wx_server_app_secret</t>
   </si>
   <si>
-    <t>系统配置</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>邮箱配置</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>web</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>web_email</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>邮箱账号</t>
   </si>
   <si>
@@ -889,108 +936,12 @@
     <t>email_port</t>
   </si>
   <si>
-    <t>is_staff</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$2b$12$Ce7eSUKIIl8DMKeDyNHyr.Dp4aesQCM70RePigRVEny1Eql31R0Cq</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>管理员</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://fastapi.tiangolo.com/img/icon-white.svg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>akura_k</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Sakura_k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>是一套开箱即用的中后台解决方案，可以作为新项目的启动模版。</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0b67fa252ad1e94f6e9fe515d5dcf37c</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ry@beidoucom.com</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>13206269804</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@163.com</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>em</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ail</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ry@beidoucom.com</t>
-  </si>
-  <si>
-    <t>$2b$12$1j53PS8lNyAdF4xv24DCx.l4FxHPe5OULqKv90yRDVEPi1lmLsxuG</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>/media/system/logo.png</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/media/system/favicon.ico</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1000,7 +951,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm:ss"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1008,8 +959,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -1020,24 +971,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1063,33 +1004,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1366,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2084,31 +2005,31 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>44844.410787036999</v>
+        <v>44862.895787037</v>
       </c>
       <c r="C13" s="1">
-        <v>44862.9241203704</v>
+        <v>44870.493113425902</v>
       </c>
       <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" t="s">
-        <v>61</v>
-      </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I13">
         <v>3</v>
       </c>
       <c r="K13">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2129,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2140,16 +2061,16 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>44862.895787037</v>
+        <v>44864.733217592599</v>
       </c>
       <c r="C14" s="1">
-        <v>44870.493113425902</v>
+        <v>44864.733217592599</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>63</v>
@@ -2158,13 +2079,13 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="I14">
         <v>3</v>
       </c>
       <c r="K14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2196,13 +2117,13 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>44864.733217592599</v>
+        <v>44862.8991550926</v>
       </c>
       <c r="C15" s="1">
-        <v>44864.733217592599</v>
+        <v>44862.9000578704</v>
       </c>
       <c r="E15" t="s">
         <v>65</v>
@@ -2217,7 +2138,7 @@
         <v>37</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -2252,13 +2173,13 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>44862.8991550926</v>
+        <v>44862.925173611096</v>
       </c>
       <c r="C16" s="1">
-        <v>44862.9000578704</v>
+        <v>44863.569282407399</v>
       </c>
       <c r="E16" t="s">
         <v>68</v>
@@ -2276,7 +2197,7 @@
         <v>13</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2308,31 +2229,28 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>44862.925173611096</v>
+        <v>44883.598217592596</v>
       </c>
       <c r="C17" s="1">
-        <v>44863.569282407399</v>
-      </c>
-      <c r="E17" t="s">
+        <v>44883.604062500002</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
         <v>71</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
         <v>72</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17">
-        <v>13</v>
-      </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2364,49 +2282,49 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>44883.598217592596</v>
+        <v>44883.6410300926</v>
       </c>
       <c r="C18" s="1">
-        <v>44883.604062500002</v>
+        <v>44883.6410300926</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I18">
         <v>7</v>
       </c>
       <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" t="s">
         <v>75</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18" t="s">
-        <v>76</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -2417,49 +2335,49 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>44883.6410300926</v>
+        <v>44883.641284722202</v>
       </c>
       <c r="C19" s="1">
-        <v>44883.6410300926</v>
+        <v>44883.641284722202</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I19">
         <v>7</v>
       </c>
       <c r="J19" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
         <v>77</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19" t="s">
-        <v>78</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -2470,49 +2388,49 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>44883.641284722202</v>
+        <v>44883.633275462998</v>
       </c>
       <c r="C20" s="1">
-        <v>44883.641284722202</v>
+        <v>44883.633275462998</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" t="s">
         <v>79</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20" t="s">
-        <v>80</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -2523,49 +2441,49 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>44883.633275462998</v>
+        <v>44883.641620370399</v>
       </c>
       <c r="C21" s="1">
-        <v>44883.633275462998</v>
+        <v>44883.641620370399</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21">
         <v>8</v>
       </c>
       <c r="J21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21" t="s">
         <v>81</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21" t="s">
-        <v>82</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -2576,28 +2494,28 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>44883.641620370399</v>
+        <v>44883.6417939815</v>
       </c>
       <c r="C22" s="1">
-        <v>44883.641620370399</v>
+        <v>44883.6417939815</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I22">
         <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2618,7 +2536,7 @@
         <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -2629,28 +2547,28 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>44883.6417939815</v>
+        <v>44883.643275463</v>
       </c>
       <c r="C23" s="1">
-        <v>44883.6417939815</v>
+        <v>44883.646527777797</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2671,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -2682,49 +2600,49 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>44883.643275463</v>
+        <v>44883.643530092602</v>
       </c>
       <c r="C24" s="1">
-        <v>44883.646527777797</v>
+        <v>44883.643530092602</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I24">
         <v>9</v>
       </c>
       <c r="J24" t="s">
+        <v>85</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24" t="s">
         <v>86</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24" t="s">
-        <v>87</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -2735,49 +2653,49 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>44883.643530092602</v>
+        <v>44883.643819444398</v>
       </c>
       <c r="C25" s="1">
-        <v>44883.643530092602</v>
+        <v>44883.643819444398</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I25">
         <v>9</v>
       </c>
       <c r="J25" t="s">
+        <v>87</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25" t="s">
         <v>88</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25" t="s">
-        <v>89</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -2788,49 +2706,49 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
-        <v>44883.643819444398</v>
+        <v>44883.644166666701</v>
       </c>
       <c r="C26" s="1">
-        <v>44883.643819444398</v>
+        <v>44883.644166666701</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I26">
         <v>9</v>
       </c>
       <c r="J26" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26" t="s">
         <v>90</v>
-      </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26" t="s">
-        <v>91</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -2841,49 +2759,49 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
-        <v>44883.644166666701</v>
+        <v>44883.644386574102</v>
       </c>
       <c r="C27" s="1">
-        <v>44883.644166666701</v>
+        <v>44883.644386574102</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I27">
         <v>9</v>
       </c>
       <c r="J27" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27" t="s">
         <v>92</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27" t="s">
-        <v>93</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -2894,49 +2812,49 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>44883.644386574102</v>
+        <v>44883.644884259302</v>
       </c>
       <c r="C28" s="1">
-        <v>44883.644386574102</v>
+        <v>44883.644884259302</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I28">
         <v>9</v>
       </c>
       <c r="J28" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" t="s">
         <v>94</v>
-      </c>
-      <c r="K28">
-        <v>4</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28" t="s">
-        <v>95</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -2947,28 +2865,31 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1">
-        <v>44883.644884259302</v>
+        <v>44973.6896180556</v>
       </c>
       <c r="C29" s="1">
-        <v>44883.644884259302</v>
+        <v>44973.690972222197</v>
+      </c>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>74</v>
-      </c>
-      <c r="I29">
-        <v>9</v>
-      </c>
-      <c r="J29" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2992,7 +2913,7 @@
         <v>97</v>
       </c>
       <c r="U29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -3000,19 +2921,16 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1">
-        <v>44973.6896180556</v>
+        <v>44973.690277777801</v>
       </c>
       <c r="C30" s="1">
-        <v>44973.690972222197</v>
-      </c>
-      <c r="D30" t="s">
+        <v>44973.691400463002</v>
+      </c>
+      <c r="E30" t="s">
         <v>98</v>
-      </c>
-      <c r="E30" t="s">
-        <v>23</v>
       </c>
       <c r="F30" t="s">
         <v>99</v>
@@ -3021,10 +2939,13 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="I30">
+        <v>38</v>
       </c>
       <c r="K30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -3048,7 +2969,7 @@
         <v>100</v>
       </c>
       <c r="U30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -3056,13 +2977,13 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
-        <v>44973.690277777801</v>
+        <v>44973.717280092598</v>
       </c>
       <c r="C31" s="1">
-        <v>44973.691400463002</v>
+        <v>44973.719930555599</v>
       </c>
       <c r="E31" t="s">
         <v>101</v>
@@ -3080,7 +3001,7 @@
         <v>38</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -3112,13 +3033,13 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1">
-        <v>44973.717280092598</v>
+        <v>44978.987083333297</v>
       </c>
       <c r="C32" s="1">
-        <v>44973.719930555599</v>
+        <v>44978.987083333297</v>
       </c>
       <c r="E32" t="s">
         <v>104</v>
@@ -3127,7 +3048,7 @@
         <v>105</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
         <v>37</v>
@@ -3136,7 +3057,7 @@
         <v>38</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3168,35 +3089,35 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1">
-        <v>44978.987083333297</v>
+        <v>44889.630127314798</v>
       </c>
       <c r="C33" s="1">
-        <v>44978.987083333297</v>
-      </c>
-      <c r="E33" t="s">
+        <v>44889.641284722202</v>
+      </c>
+      <c r="D33" t="s">
         <v>107</v>
       </c>
       <c r="F33" t="s">
         <v>108</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>37</v>
-      </c>
-      <c r="I33">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K33">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
+      <c r="M33" t="s">
+        <v>109</v>
+      </c>
       <c r="N33">
         <v>0</v>
       </c>
@@ -3213,10 +3134,10 @@
         <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -3224,34 +3145,34 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44889.630659722199</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44889.641111111101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34">
         <v>68</v>
       </c>
-      <c r="B34" s="1">
-        <v>44889.630127314798</v>
-      </c>
-      <c r="C34" s="1">
-        <v>44889.641284722202</v>
-      </c>
-      <c r="D34" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" t="s">
-        <v>111</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>25</v>
-      </c>
       <c r="K34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>0</v>
-      </c>
-      <c r="M34" t="s">
-        <v>112</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -3272,7 +3193,7 @@
         <v>113</v>
       </c>
       <c r="U34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -3280,13 +3201,13 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B35" s="1">
-        <v>44889.630659722199</v>
+        <v>45102.614305555602</v>
       </c>
       <c r="C35" s="1">
-        <v>44889.641111111101</v>
+        <v>45102.614305555602</v>
       </c>
       <c r="E35" t="s">
         <v>114</v>
@@ -3297,14 +3218,14 @@
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35" t="s">
-        <v>37</v>
+      <c r="H35" s="4">
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3334,8 +3255,64 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:22">
+      <c r="A36">
+        <v>74</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45105.454143518502</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45105.454143518502</v>
+      </c>
+      <c r="E36" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>13</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36" t="s">
+        <v>118</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3367,16 +3344,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -3402,10 +3379,10 @@
         <v>44843.627476851798</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3421,17 +3398,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3439,176 +3416,110 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.140625" customWidth="1"/>
-    <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44784.845185185201</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44888.896111111098</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10">
-        <v>44784.845185185201</v>
-      </c>
-      <c r="C2" s="10">
-        <v>44888.896111111098</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="8">
-        <v>1</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11">
-        <v>45061.728391203702</v>
-      </c>
-      <c r="C3" s="11">
-        <v>45061.730069444442</v>
-      </c>
-      <c r="D3" s="8">
-        <v>13206269804</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="13">
-        <v>1</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="N3" s="11">
-        <v>45061.729930555557</v>
-      </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="https://fastapi.管理员.com/img/icon-white.svg" xr:uid="{123EAE1A-000B-476D-8B77-383D7C062274}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{7A742420-628F-4D78-8429-5535AE30F689}"/>
-  </hyperlinks>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3623,14 +3534,14 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>136</v>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3645,7 +3556,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -3653,10 +3564,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3680,13 +3591,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -3709,10 +3620,10 @@
         <v>44842.581435185202</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3732,10 +3643,10 @@
         <v>44842.581620370402</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -3755,10 +3666,10 @@
         <v>44898.991770833301</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3778,10 +3689,10 @@
         <v>44898.992488425902</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3790,18 +3701,44 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45102.705092592601</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45107.391307870399</v>
+      </c>
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3824,13 +3761,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -3839,10 +3776,10 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="J1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="K1" t="s">
         <v>19</v>
@@ -3853,17 +3790,20 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>44841.503692129598</v>
+        <v>44841.505358796298</v>
       </c>
       <c r="C2" s="1">
-        <v>44841.503692129598</v>
+        <v>44841.505578703698</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="G2">
         <v>0</v>
       </c>
@@ -3871,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
@@ -3882,13 +3822,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>44841.505358796298</v>
+        <v>44842.580231481501</v>
       </c>
       <c r="C3" s="1">
-        <v>44841.505578703698</v>
+        <v>44842.580231481501</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3900,13 +3840,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -3914,31 +3854,31 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>44842.580231481501</v>
+        <v>44842.586979166699</v>
       </c>
       <c r="C4" s="1">
-        <v>44842.580231481501</v>
+        <v>44842.5872453704</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -3946,16 +3886,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>44842.586979166699</v>
+        <v>44842.587083333303</v>
       </c>
       <c r="C5" s="1">
-        <v>44842.5872453704</v>
+        <v>44842.587083333303</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3964,13 +3904,13 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -3978,13 +3918,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>44842.587083333303</v>
+        <v>44842.587175925903</v>
       </c>
       <c r="C6" s="1">
-        <v>44842.587083333303</v>
+        <v>44842.587175925903</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3996,13 +3936,13 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -4010,31 +3950,31 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>44842.587175925903</v>
+        <v>44898.9920486111</v>
       </c>
       <c r="C7" s="1">
-        <v>44842.587175925903</v>
+        <v>44898.9920486111</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -4042,13 +3982,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>44898.9920486111</v>
+        <v>44898.992210648197</v>
       </c>
       <c r="C8" s="1">
-        <v>44898.9920486111</v>
+        <v>44898.992210648197</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -4060,13 +4000,13 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -4074,31 +4014,31 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>44898.992210648197</v>
+        <v>44898.9926388889</v>
       </c>
       <c r="C9" s="1">
-        <v>44898.992210648197</v>
+        <v>44898.9926388889</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -4106,13 +4046,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>44898.9926388889</v>
+        <v>44898.992835648198</v>
       </c>
       <c r="C10" s="1">
-        <v>44898.9926388889</v>
+        <v>44898.992835648198</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4124,13 +4064,13 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4138,31 +4078,31 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>44898.992835648198</v>
+        <v>44980.950659722199</v>
       </c>
       <c r="C11" s="1">
-        <v>44898.992835648198</v>
+        <v>44980.953773148103</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4170,38 +4110,102 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>44980.950659722199</v>
+        <v>45102.705671296302</v>
       </c>
       <c r="C12" s="1">
-        <v>44980.953773148103</v>
+        <v>45103.661284722199</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" t="s">
+        <v>170</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45102.706574074102</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45102.706574074102</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J13" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45102.706724536998</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45103.661400463003</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="I12" t="s">
-        <v>161</v>
-      </c>
-      <c r="J12" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12">
+      <c r="I14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J14" t="s">
+        <v>174</v>
+      </c>
+      <c r="L14">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4242,16 +4246,16 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="I1" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="J1" t="s">
         <v>11</v>
@@ -4271,19 +4275,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I2" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -4303,19 +4307,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4335,19 +4339,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -4367,19 +4371,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -4399,19 +4403,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I6" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -4431,19 +4435,19 @@
         <v>44873.393229166701</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="I7" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -4463,19 +4467,19 @@
         <v>44873.393449074101</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="I8" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -4495,7 +4499,7 @@
         <v>44882.803460648101</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
@@ -4507,7 +4511,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -4527,19 +4531,19 @@
         <v>44971.953680555598</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="I10" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -4558,20 +4562,20 @@
       <c r="C11" s="1">
         <v>44971.953680555598</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>263</v>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>265</v>
+      <c r="H11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -4581,7 +4585,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4590,8 +4594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4599,7 +4603,7 @@
     <col min="2" max="3" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" customWidth="1"/>
     <col min="8" max="8" width="98" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4617,19 +4621,19 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="H1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="J1" t="s">
         <v>11</v>
@@ -4649,13 +4653,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>280</v>
+        <v>206</v>
+      </c>
+      <c r="G2" t="s">
+        <v>207</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -4678,10 +4682,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>209</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>292</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -4704,13 +4711,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>281</v>
+        <v>211</v>
+      </c>
+      <c r="G4" t="s">
+        <v>212</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -4733,10 +4740,13 @@
         <v>44942.757025462997</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>214</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -4759,10 +4769,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>199</v>
+        <v>216</v>
+      </c>
+      <c r="G6" t="s">
+        <v>217</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -4785,10 +4798,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="F7" t="s">
-        <v>201</v>
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>220</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -4811,13 +4827,13 @@
         <v>44887.691469907397</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="H8" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -4840,13 +4856,13 @@
         <v>44965.452013888898</v>
       </c>
       <c r="E9" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -4869,13 +4885,13 @@
         <v>44869.679618055503</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="G10" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -4898,10 +4914,10 @@
         <v>44873.394305555601</v>
       </c>
       <c r="E11" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -4924,10 +4940,10 @@
         <v>44873.394861111097</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="F12" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -4950,13 +4966,13 @@
         <v>44873.397835648102</v>
       </c>
       <c r="E13" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="F13" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="H13" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="I13">
         <v>6</v>
@@ -4979,13 +4995,13 @@
         <v>44873.404872685198</v>
       </c>
       <c r="E14" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="F14" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H14" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -5008,13 +5024,13 @@
         <v>44873.948194444398</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="F15" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="G15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -5037,13 +5053,13 @@
         <v>44873.948611111096</v>
       </c>
       <c r="E16" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="F16" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="G16" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="I16">
         <v>6</v>
@@ -5066,13 +5082,13 @@
         <v>44880.940173611103</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="H17" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -5095,13 +5111,13 @@
         <v>44880.941412036998</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="F18" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="H18" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -5124,16 +5140,13 @@
         <v>44882.8044212963</v>
       </c>
       <c r="E19" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="F19" t="s">
-        <v>230</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="H19" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="I19">
         <v>8</v>
@@ -5156,16 +5169,16 @@
         <v>44882.805381944403</v>
       </c>
       <c r="E20" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="G20" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="H20" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="I20">
         <v>8</v>
@@ -5188,16 +5201,16 @@
         <v>44882.805740740703</v>
       </c>
       <c r="E21" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="F21" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="G21" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="H21" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="I21">
         <v>8</v>
@@ -5220,16 +5233,16 @@
         <v>44882.814594907402</v>
       </c>
       <c r="E22" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="F22" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="G22" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="H22" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="I22">
         <v>8</v>
@@ -5252,16 +5265,16 @@
         <v>44882.815324074101</v>
       </c>
       <c r="E23" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="F23" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="G23" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="H23" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="I23">
         <v>8</v>
@@ -5284,16 +5297,16 @@
         <v>44882.816689814797</v>
       </c>
       <c r="E24" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="F24" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="G24" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="H24" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="I24">
         <v>8</v>
@@ -5316,13 +5329,13 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E25" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="F25" t="s">
-        <v>253</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>283</v>
+        <v>272</v>
+      </c>
+      <c r="G25" t="s">
+        <v>273</v>
       </c>
       <c r="I25">
         <v>9</v>
@@ -5345,10 +5358,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E26" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="F26" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="I26">
         <v>9</v>
@@ -5371,10 +5384,13 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E27" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="F27" t="s">
-        <v>257</v>
+        <v>277</v>
+      </c>
+      <c r="G27" t="s">
+        <v>278</v>
       </c>
       <c r="I27">
         <v>9</v>
@@ -5397,10 +5413,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E28" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="F28" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="I28">
         <v>9</v>
@@ -5423,10 +5439,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E29" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="F29" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="I29">
         <v>9</v>
@@ -5448,15 +5464,13 @@
       <c r="C30" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>266</v>
+      <c r="E30" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="F30" t="s">
-        <v>267</v>
-      </c>
-      <c r="G30" s="4" t="s">
         <v>284</v>
       </c>
+      <c r="G30" s="3"/>
       <c r="I30">
         <v>10</v>
       </c>
@@ -5477,13 +5491,13 @@
       <c r="C31" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>268</v>
+      <c r="E31" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="F31" t="s">
-        <v>269</v>
-      </c>
-      <c r="G31" s="7"/>
+        <v>286</v>
+      </c>
+      <c r="G31" s="4"/>
       <c r="I31">
         <v>10</v>
       </c>
@@ -5504,14 +5518,14 @@
       <c r="C32" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>270</v>
+      <c r="E32" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="F32" t="s">
-        <v>271</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>272</v>
+        <v>288</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="I32">
         <v>10</v>
@@ -5533,13 +5547,13 @@
       <c r="C33" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>273</v>
+      <c r="E33" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="F33" t="s">
-        <v>274</v>
-      </c>
-      <c r="G33" s="5">
+        <v>291</v>
+      </c>
+      <c r="G33" s="4">
         <v>25</v>
       </c>
       <c r="I33">
@@ -5553,11 +5567,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="G25" r:id="rId1" xr:uid="{AB2F913A-073D-428C-A298-E0563D2AAD28}"/>
-    <hyperlink ref="G30" r:id="rId2" xr:uid="{AB4E9E47-7019-4F3A-9F9B-172570F9F010}"/>
-  </hyperlinks>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
🐞 Fix(Fix migration database bugs): 修复迁移数据库BUG
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitpush\Sakura_K\scripts\initialize\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\冉勇\Desktop\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70C12F-E3E8-4C98-AF76-D209698B32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18EBE16-25E3-4645-875D-E9D3EE1C6CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1740" windowWidth="29040" windowHeight="16440" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="298">
   <si>
     <t>title</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>图片资源</t>
-  </si>
-  <si>
-    <t>views/vadmin/resource/images/index</t>
   </si>
   <si>
     <t>images</t>
@@ -976,7 +973,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1008,7 +1005,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>-</t>
     </r>
@@ -1429,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1750,7 +1747,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1806,7 +1803,7 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -1862,7 +1859,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>
@@ -1918,7 +1915,7 @@
         <v>47</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -1974,7 +1971,7 @@
         <v>49</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" t="s">
         <v>50</v>
@@ -2086,7 +2083,7 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -2142,7 +2139,7 @@
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -2198,7 +2195,7 @@
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E14" t="s">
         <v>58</v>
@@ -2946,7 +2943,7 @@
         <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E28" t="s">
         <v>88</v>
@@ -3002,7 +2999,7 @@
         <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E29" t="s">
         <v>90</v>
@@ -3058,7 +3055,7 @@
         <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E30" t="s">
         <v>92</v>
@@ -3170,7 +3167,7 @@
         <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
@@ -3226,7 +3223,7 @@
         <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E33" t="s">
         <v>100</v>
@@ -3282,7 +3279,7 @@
         <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E34" t="s">
         <v>100</v>
@@ -3553,10 +3550,10 @@
         <v>111</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -3601,62 +3598,6 @@
         <v>45183.466342592597</v>
       </c>
       <c r="V39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="A40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" t="s">
-        <v>112</v>
-      </c>
-      <c r="E40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>38</v>
-      </c>
-      <c r="J40">
-        <v>79</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>80</v>
-      </c>
-      <c r="S40" s="1">
-        <v>45163.581469907404</v>
-      </c>
-      <c r="T40" s="1">
-        <v>45163.581469907404</v>
-      </c>
-      <c r="V40">
         <v>0</v>
       </c>
     </row>
@@ -3670,7 +3611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -3703,22 +3644,22 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
         <v>261</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>262</v>
       </c>
-      <c r="I1" t="s">
-        <v>263</v>
-      </c>
       <c r="J1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3738,10 +3679,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3770,10 +3711,10 @@
         <v>3</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3802,10 +3743,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -3834,10 +3775,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -3866,10 +3807,10 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
+        <v>266</v>
+      </c>
+      <c r="H6" t="s">
         <v>267</v>
-      </c>
-      <c r="H6" t="s">
-        <v>268</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3898,10 +3839,10 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
+        <v>268</v>
+      </c>
+      <c r="H7" t="s">
         <v>269</v>
-      </c>
-      <c r="H7" t="s">
-        <v>270</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -3930,10 +3871,10 @@
         <v>4</v>
       </c>
       <c r="G8" t="s">
+        <v>270</v>
+      </c>
+      <c r="H8" t="s">
         <v>271</v>
-      </c>
-      <c r="H8" t="s">
-        <v>272</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -3978,16 +3919,16 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -4013,10 +3954,10 @@
         <v>44843.627476851798</v>
       </c>
       <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>119</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -4041,8 +3982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4070,34 +4011,34 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
         <v>120</v>
       </c>
-      <c r="E1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>122</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J1" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>124</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>125</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>126</v>
-      </c>
-      <c r="M1" t="s">
-        <v>127</v>
       </c>
       <c r="N1" t="s">
         <v>20</v>
@@ -4106,7 +4047,7 @@
         <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -4123,13 +4064,13 @@
         <v>15020221010</v>
       </c>
       <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
         <v>129</v>
-      </c>
-      <c r="F2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" t="s">
-        <v>130</v>
       </c>
       <c r="I2" t="s">
         <v>38</v>
@@ -4141,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M2" s="1"/>
       <c r="O2">
@@ -4152,6 +4093,12 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="136.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45197.896111111113</v>
+      </c>
       <c r="C3" s="1">
         <v>45197.896111111113</v>
       </c>
@@ -4159,17 +4106,17 @@
         <v>13206269804</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>290</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
@@ -4180,7 +4127,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M3" s="1"/>
       <c r="O3">
@@ -4215,10 +4162,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
         <v>132</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4241,7 +4188,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4265,13 +4212,13 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>135</v>
-      </c>
-      <c r="F1" t="s">
-        <v>136</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -4294,10 +4241,10 @@
         <v>44842.581435185202</v>
       </c>
       <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" t="s">
         <v>137</v>
-      </c>
-      <c r="E2" t="s">
-        <v>138</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -4317,10 +4264,10 @@
         <v>44842.581620370402</v>
       </c>
       <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" t="s">
         <v>139</v>
-      </c>
-      <c r="E3" t="s">
-        <v>140</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -4340,10 +4287,10 @@
         <v>44898.991770833301</v>
       </c>
       <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="s">
         <v>141</v>
-      </c>
-      <c r="E4" t="s">
-        <v>142</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -4363,10 +4310,10 @@
         <v>44898.992488425902</v>
       </c>
       <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
         <v>143</v>
-      </c>
-      <c r="E5" t="s">
-        <v>144</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -4386,13 +4333,13 @@
         <v>45107.391307870399</v>
       </c>
       <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
         <v>145</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>146</v>
-      </c>
-      <c r="F6" t="s">
-        <v>147</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4435,13 +4382,13 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
         <v>148</v>
       </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -4450,10 +4397,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" t="s">
         <v>150</v>
-      </c>
-      <c r="J1" t="s">
-        <v>151</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -4485,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J2" t="s">
         <v>27</v>
@@ -4517,7 +4464,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J3" t="s">
         <v>38</v>
@@ -4549,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
@@ -4581,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -4613,7 +4560,7 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
         <v>60</v>
@@ -4645,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J7" t="s">
         <v>27</v>
@@ -4677,7 +4624,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -4709,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
@@ -4741,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J10" t="s">
         <v>38</v>
@@ -4773,7 +4720,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J11" t="s">
         <v>60</v>
@@ -4805,10 +4752,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
+        <v>161</v>
+      </c>
+      <c r="J12" t="s">
         <v>162</v>
-      </c>
-      <c r="J12" t="s">
-        <v>163</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4837,10 +4784,10 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
+        <v>163</v>
+      </c>
+      <c r="J13" t="s">
         <v>164</v>
-      </c>
-      <c r="J13" t="s">
-        <v>165</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -4869,10 +4816,10 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J14" t="s">
         <v>166</v>
-      </c>
-      <c r="J14" t="s">
-        <v>167</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -4920,16 +4867,16 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
         <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>170</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -4952,16 +4899,16 @@
         <v>53</v>
       </c>
       <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>171</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>172</v>
-      </c>
-      <c r="I2" t="s">
-        <v>173</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -4984,16 +4931,16 @@
         <v>53</v>
       </c>
       <c r="F3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" t="s">
         <v>174</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I3" t="s">
-        <v>175</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -5016,16 +4963,16 @@
         <v>53</v>
       </c>
       <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" t="s">
         <v>176</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" t="s">
-        <v>177</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -5048,16 +4995,16 @@
         <v>53</v>
       </c>
       <c r="F5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" t="s">
         <v>178</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>172</v>
-      </c>
-      <c r="I5" t="s">
-        <v>179</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -5080,16 +5027,16 @@
         <v>53</v>
       </c>
       <c r="F6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s">
         <v>180</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>172</v>
-      </c>
-      <c r="I6" t="s">
-        <v>181</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -5109,19 +5056,19 @@
         <v>44873.393229166701</v>
       </c>
       <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" t="s">
         <v>182</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>183</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>184</v>
-      </c>
-      <c r="I7" t="s">
-        <v>185</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -5141,19 +5088,19 @@
         <v>44873.393449074101</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I8" t="s">
         <v>186</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>184</v>
-      </c>
-      <c r="I8" t="s">
-        <v>187</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -5173,7 +5120,7 @@
         <v>44882.803460648101</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -5185,7 +5132,7 @@
         <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -5208,16 +5155,16 @@
         <v>53</v>
       </c>
       <c r="F10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s">
         <v>190</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" t="s">
-        <v>191</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -5240,16 +5187,16 @@
         <v>53</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I11" t="s">
         <v>192</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" t="s">
-        <v>193</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -5295,19 +5242,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" t="s">
         <v>194</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>195</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" t="s">
         <v>196</v>
-      </c>
-      <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>197</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -5327,13 +5274,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" t="s">
-        <v>199</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -5356,13 +5303,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" t="s">
         <v>200</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>201</v>
-      </c>
-      <c r="G3" t="s">
-        <v>202</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -5385,10 +5332,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
         <v>203</v>
-      </c>
-      <c r="F4" t="s">
-        <v>204</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -5411,13 +5358,13 @@
         <v>44942.757025462997</v>
       </c>
       <c r="E5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" t="s">
         <v>205</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>206</v>
-      </c>
-      <c r="G5" t="s">
-        <v>207</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -5440,10 +5387,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" t="s">
         <v>208</v>
-      </c>
-      <c r="F6" t="s">
-        <v>209</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -5466,10 +5413,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" t="s">
         <v>210</v>
-      </c>
-      <c r="F7" t="s">
-        <v>211</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -5492,13 +5439,13 @@
         <v>44887.691469907397</v>
       </c>
       <c r="E8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" t="s">
         <v>212</v>
-      </c>
-      <c r="F8" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" t="s">
-        <v>213</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -5521,13 +5468,13 @@
         <v>44965.452013888898</v>
       </c>
       <c r="E9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" t="s">
         <v>214</v>
-      </c>
-      <c r="F9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" t="s">
-        <v>215</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -5550,13 +5497,13 @@
         <v>44869.679618055503</v>
       </c>
       <c r="E10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
         <v>180</v>
       </c>
-      <c r="F10" t="s">
-        <v>181</v>
-      </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -5579,10 +5526,10 @@
         <v>44873.394305555601</v>
       </c>
       <c r="E11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" t="s">
         <v>217</v>
-      </c>
-      <c r="F11" t="s">
-        <v>218</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -5605,10 +5552,10 @@
         <v>44873.394861111097</v>
       </c>
       <c r="E12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" t="s">
         <v>219</v>
-      </c>
-      <c r="F12" t="s">
-        <v>220</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -5631,13 +5578,13 @@
         <v>44873.397835648102</v>
       </c>
       <c r="E13" t="s">
+        <v>220</v>
+      </c>
+      <c r="F13" t="s">
         <v>221</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>222</v>
-      </c>
-      <c r="H13" t="s">
-        <v>223</v>
       </c>
       <c r="I13">
         <v>6</v>
@@ -5660,13 +5607,13 @@
         <v>44873.404872685198</v>
       </c>
       <c r="E14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" t="s">
         <v>224</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>225</v>
-      </c>
-      <c r="H14" t="s">
-        <v>226</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -5689,13 +5636,13 @@
         <v>44873.948194444398</v>
       </c>
       <c r="E15" t="s">
+        <v>226</v>
+      </c>
+      <c r="F15" t="s">
         <v>227</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>228</v>
-      </c>
-      <c r="G15" t="s">
-        <v>229</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -5718,13 +5665,13 @@
         <v>44873.948611111096</v>
       </c>
       <c r="E16" t="s">
+        <v>229</v>
+      </c>
+      <c r="F16" t="s">
         <v>230</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>231</v>
-      </c>
-      <c r="G16" t="s">
-        <v>232</v>
       </c>
       <c r="I16">
         <v>6</v>
@@ -5747,13 +5694,13 @@
         <v>44880.940173611103</v>
       </c>
       <c r="E17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17" t="s">
         <v>233</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>234</v>
-      </c>
-      <c r="H17" t="s">
-        <v>235</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -5776,13 +5723,13 @@
         <v>44880.941412036998</v>
       </c>
       <c r="E18" t="s">
+        <v>235</v>
+      </c>
+      <c r="F18" t="s">
         <v>236</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>237</v>
-      </c>
-      <c r="H18" t="s">
-        <v>238</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -5805,10 +5752,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" t="s">
         <v>239</v>
-      </c>
-      <c r="F19" t="s">
-        <v>240</v>
       </c>
       <c r="I19">
         <v>9</v>
@@ -5831,10 +5778,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E20" t="s">
+        <v>240</v>
+      </c>
+      <c r="F20" t="s">
         <v>241</v>
-      </c>
-      <c r="F20" t="s">
-        <v>242</v>
       </c>
       <c r="I20">
         <v>9</v>
@@ -5857,10 +5804,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F21" t="s">
         <v>243</v>
-      </c>
-      <c r="F21" t="s">
-        <v>244</v>
       </c>
       <c r="G21" s="2"/>
       <c r="I21">
@@ -5884,10 +5831,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E22" t="s">
+        <v>244</v>
+      </c>
+      <c r="F22" t="s">
         <v>245</v>
-      </c>
-      <c r="F22" t="s">
-        <v>246</v>
       </c>
       <c r="I22">
         <v>9</v>
@@ -5910,10 +5857,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E23" t="s">
+        <v>246</v>
+      </c>
+      <c r="F23" t="s">
         <v>247</v>
-      </c>
-      <c r="F23" t="s">
-        <v>248</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -5936,10 +5883,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F24" t="s">
         <v>249</v>
-      </c>
-      <c r="F24" t="s">
-        <v>250</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24">
@@ -5963,10 +5910,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F25" t="s">
         <v>251</v>
-      </c>
-      <c r="F25" t="s">
-        <v>252</v>
       </c>
       <c r="G25" s="5"/>
       <c r="I25">
@@ -5990,13 +5937,13 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F26" t="s">
         <v>253</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -6019,10 +5966,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F27" t="s">
         <v>256</v>
-      </c>
-      <c r="F27" t="s">
-        <v>257</v>
       </c>
       <c r="G27" s="5">
         <v>25</v>
@@ -6079,16 +6026,16 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
         <v>258</v>
-      </c>
-      <c r="H1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6105,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -6131,7 +6078,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
🐞 Fix(Fix the create assignment permission drop-down bug and optimize init.xls): 修复创建分配权限下拉bug，优化init.xls
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\冉勇\Desktop\Sakura_K\scripts\initialize\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitpush\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18EBE16-25E3-4645-875D-E9D3EE1C6CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EE556-345F-4EC3-84A1-48D5837A808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1740" windowWidth="29040" windowHeight="16440" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1740" windowWidth="29040" windowHeight="16440" tabRatio="887" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="294">
   <si>
     <t>title</t>
   </si>
@@ -187,9 +187,6 @@
     <t>日志管理</t>
   </si>
   <si>
-    <t>record</t>
-  </si>
-  <si>
     <t>系统配置</t>
   </si>
   <si>
@@ -400,6 +397,9 @@
     <t>avatar</t>
   </si>
   <si>
+    <t>gender</t>
+  </si>
+  <si>
     <t>is_active</t>
   </si>
   <si>
@@ -413,12 +413,6 @@
   </si>
   <si>
     <t>is_staff</t>
-  </si>
-  <si>
-    <t>kinit</t>
-  </si>
-  <si>
-    <t>$2b$12$Ce7eSUKIIl8DMKeDyNHyr.Dp4aesQCM70RePigRVEny1Eql31R0Cq</t>
   </si>
   <si>
     <t>127.0.0.1</t>
@@ -851,9 +845,6 @@
     <t>view_number</t>
   </si>
   <si>
-    <t>&lt;p&gt;是的，是在若依-移动端的基础上进行的二次开发，在此感谢若依团队！二次开发中我们重新将接口请求改为 luch-request 组件，项目结构也有所改动，并且加入了 uView UI 组件，uni-simple-router 路由拦截。&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;开源&lt;/p&gt;</t>
   </si>
   <si>
@@ -879,68 +870,55 @@
   </si>
   <si>
     <t>views/Dashboard/Analysis/Analysis</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Auth/Menu/Menu</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Auth/Role/Role</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Auth/User/User</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Dict/Dict</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Settings/Settings</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Record/Login/Login</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Record/Operation/Operation</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Help/IssueCategory/IssueCategory</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Help/Issue/Issue</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Help/Issue/components/Write</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Screen/Air/Air</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Task/Task</t>
+  </si>
+  <si>
+    <t>views/Vadmin/System/Record/Task/Task</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Resource/Image/Image</t>
+  </si>
+  <si>
+    <t>tdesign:catalog</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>views/Vadmin/Auth/Menu/Menu</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Auth/Role/Role</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>views/Vadmin/Auth/User/User</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Dict/Dict</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Settings/Settings</t>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Record/Login/Login</t>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Record/Operation/Operation</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Help/IssueCategory/IssueCategory</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Help/Issue/Issue</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Help/Issue/components/Write</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Screen/Air/Air</t>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Task/Task</t>
-  </si>
-  <si>
-    <t>views/Vadmin/System/Record/Task/Task</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Resource/Image/Image</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>$2b$12$7EHv05AHcpnRTmf342XkGe0bacfVF.m04mpL3cnFgt.Ja7P7UVjpu</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>冉勇</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://ran-oss-yong.oss-cn-shenzhen.aliyuncs.com/avatar.gif</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>gender</t>
+    <t>/record</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -955,6 +933,14 @@
       </rPr>
       <t>akura_K</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>冉勇</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ran-oss-yong.oss-cn-shenzhen.aliyuncs.com/avatar.gif</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -984,53 +970,6 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>问题</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sakura_K </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>是使用若依</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>移动端进行的二次开发吗？</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Sakura_K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>开源吗？</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1052,7 +991,7 @@
   </si>
   <si>
     <r>
-      <t>Sakura_K</t>
+      <t xml:space="preserve">Sakura </t>
     </r>
     <r>
       <rPr>
@@ -1061,12 +1000,15 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>源码地址多少？</t>
+      <t>问题</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">target="_blank"&gt;https://github.com/ranyong1997/Sakura_K&lt;/a&gt; </t>
+    <t>$2b$12$O7zTfpCO8E8URHgJPtxMhOETctVyPggHEN658s7GEsoFt3NbXGjsG</t>
+  </si>
+  <si>
+    <t>ranyong</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1088,14 +1030,12 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1428,20 +1368,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="19" max="20" width="20" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="19" max="20" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -1746,8 +1682,8 @@
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>272</v>
+      <c r="D6" t="s">
+        <v>269</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1803,7 +1739,7 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -1858,8 +1794,8 @@
       <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>274</v>
+      <c r="D8" t="s">
+        <v>271</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>
@@ -1914,8 +1850,8 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>275</v>
+      <c r="D9" t="s">
+        <v>272</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -1970,8 +1906,8 @@
       <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>276</v>
+      <c r="D10" t="s">
+        <v>273</v>
       </c>
       <c r="E10" t="s">
         <v>50</v>
@@ -2026,11 +1962,14 @@
       <c r="A11" t="s">
         <v>51</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
-        <v>52</v>
+      <c r="E11" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2039,14 +1978,11 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="I11" t="s">
         <v>27</v>
       </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
       <c r="L11">
         <v>0</v>
       </c>
@@ -2080,13 +2016,13 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2136,13 +2072,13 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>278</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2192,13 +2128,13 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>279</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2248,25 +2184,25 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
         <v>59</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>60</v>
       </c>
       <c r="J15">
         <v>7</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2301,7 +2237,7 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2313,13 +2249,13 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16">
         <v>7</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2354,7 +2290,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -2366,13 +2302,13 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17">
         <v>7</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2407,7 +2343,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2419,13 +2355,13 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18">
         <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2460,7 +2396,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2472,13 +2408,13 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19">
         <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2513,7 +2449,7 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2525,13 +2461,13 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20">
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2566,7 +2502,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2578,13 +2514,13 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J21">
         <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2619,7 +2555,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2631,13 +2567,13 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22">
         <v>9</v>
       </c>
       <c r="K22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2672,7 +2608,7 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2684,13 +2620,13 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23">
         <v>9</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2725,7 +2661,7 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2737,13 +2673,13 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J24">
         <v>9</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2778,7 +2714,7 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2790,13 +2726,13 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25">
         <v>9</v>
       </c>
       <c r="K25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2831,7 +2767,7 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2843,13 +2779,13 @@
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J26">
         <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2884,16 +2820,16 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" t="s">
-        <v>85</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2940,13 +2876,13 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>277</v>
+      </c>
+      <c r="E28" t="s">
         <v>87</v>
-      </c>
-      <c r="D28" t="s">
-        <v>280</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2996,13 +2932,13 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E29" t="s">
         <v>89</v>
-      </c>
-      <c r="D29" t="s">
-        <v>281</v>
-      </c>
-      <c r="E29" t="s">
-        <v>90</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3052,13 +2988,13 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>279</v>
+      </c>
+      <c r="E30" t="s">
         <v>91</v>
-      </c>
-      <c r="D30" t="s">
-        <v>282</v>
-      </c>
-      <c r="E30" t="s">
-        <v>92</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -3108,16 +3044,16 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
         <v>93</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>94</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>95</v>
-      </c>
-      <c r="E31" t="s">
-        <v>96</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3164,13 +3100,13 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>280</v>
+      </c>
+      <c r="E32" t="s">
         <v>97</v>
-      </c>
-      <c r="D32" t="s">
-        <v>283</v>
-      </c>
-      <c r="E32" t="s">
-        <v>98</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -3220,13 +3156,13 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>281</v>
+      </c>
+      <c r="E33" t="s">
         <v>99</v>
-      </c>
-      <c r="D33" t="s">
-        <v>284</v>
-      </c>
-      <c r="E33" t="s">
-        <v>100</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -3276,13 +3212,13 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -3332,7 +3268,7 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -3344,13 +3280,13 @@
         <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J35">
         <v>7</v>
       </c>
       <c r="K35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3385,7 +3321,7 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -3397,13 +3333,13 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J36">
         <v>8</v>
       </c>
       <c r="K36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -3438,7 +3374,7 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -3450,13 +3386,13 @@
         <v>6</v>
       </c>
       <c r="I37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J37">
         <v>9</v>
       </c>
       <c r="K37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -3491,16 +3427,16 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
         <v>108</v>
-      </c>
-      <c r="B38" t="s">
-        <v>109</v>
       </c>
       <c r="D38" t="s">
         <v>25</v>
       </c>
       <c r="E38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -3547,13 +3483,13 @@
     </row>
     <row r="39" spans="1:22">
       <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>283</v>
+      </c>
+      <c r="E39" t="s">
         <v>111</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="E39" t="s">
-        <v>112</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -3609,10 +3545,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3644,45 +3580,45 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" t="s">
         <v>260</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>261</v>
-      </c>
-      <c r="I1" t="s">
-        <v>262</v>
       </c>
       <c r="J1" t="s">
         <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>44984.657164351898</v>
+        <v>44984.657337962999</v>
       </c>
       <c r="C2" s="1">
-        <v>45142.737500000003</v>
+        <v>45142.7374305556</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3696,25 +3632,25 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>44984.657337962999</v>
+        <v>44984.657453703701</v>
       </c>
       <c r="C3" s="1">
-        <v>45142.7374305556</v>
+        <v>45142.737453703703</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3728,25 +3664,25 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>44984.657453703701</v>
+        <v>44984.657719907402</v>
       </c>
       <c r="C4" s="1">
-        <v>45142.737453703703</v>
+        <v>45141.021805555603</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>295</v>
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>263</v>
       </c>
       <c r="H4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -3760,25 +3696,25 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>44984.657581018502</v>
+        <v>44984.657847222203</v>
       </c>
       <c r="C5" s="1">
-        <v>45142.737476851798</v>
+        <v>45129.748043981497</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>297</v>
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>265</v>
+      </c>
+      <c r="H5" t="s">
+        <v>266</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -3792,25 +3728,25 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
-        <v>44984.657719907402</v>
+        <v>44984.657962963</v>
       </c>
       <c r="C6" s="1">
-        <v>45141.021805555603</v>
+        <v>45142.737407407403</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3819,70 +3755,6 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44984.657847222203</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45129.748043981497</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>268</v>
-      </c>
-      <c r="H7" t="s">
-        <v>269</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44984.657962963</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45142.737407407403</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>270</v>
-      </c>
-      <c r="H8" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
         <v>1</v>
       </c>
     </row>
@@ -3919,16 +3791,16 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>115</v>
-      </c>
-      <c r="G1" t="s">
-        <v>116</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -3954,10 +3826,10 @@
         <v>44843.627476851798</v>
       </c>
       <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
         <v>117</v>
-      </c>
-      <c r="E2" t="s">
-        <v>118</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3980,10 +3852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4011,22 +3883,22 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
         <v>119</v>
       </c>
-      <c r="E1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>122</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="J1" t="s">
         <v>123</v>
@@ -4050,103 +3922,57 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" ht="136.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44784.845185185201</v>
+        <v>45197.896111111113</v>
       </c>
       <c r="C2" s="1">
-        <v>44888.896111111098</v>
+        <v>45197.896111111113</v>
       </c>
       <c r="D2">
-        <v>15020221010</v>
-      </c>
-      <c r="E2" t="s">
+        <v>13206269804</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>128</v>
-      </c>
-      <c r="F2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>130</v>
       </c>
       <c r="M2" s="1"/>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="136.5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45197.896111111113</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45197.896111111113</v>
-      </c>
-      <c r="D3">
-        <v>13206269804</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>130</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{51B36D6D-3FF9-4A3C-81C4-1D173690B145}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{F8AEA984-9637-4FAE-8645-FAC22C399F20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="I2:P2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4162,10 +3988,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4188,7 +4014,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4212,13 +4038,13 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
         <v>133</v>
-      </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" t="s">
-        <v>135</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -4241,10 +4067,10 @@
         <v>44842.581435185202</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -4264,10 +4090,10 @@
         <v>44842.581620370402</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -4287,10 +4113,10 @@
         <v>44898.991770833301</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -4310,10 +4136,10 @@
         <v>44898.992488425902</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -4333,13 +4159,13 @@
         <v>45107.391307870399</v>
       </c>
       <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" t="s">
         <v>144</v>
-      </c>
-      <c r="E6" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" t="s">
-        <v>146</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4359,7 +4185,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4382,13 +4208,13 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -4397,10 +4223,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -4432,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J2" t="s">
         <v>27</v>
@@ -4464,7 +4290,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J3" t="s">
         <v>38</v>
@@ -4496,7 +4322,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
@@ -4528,7 +4354,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -4560,10 +4386,10 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -4592,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J7" t="s">
         <v>27</v>
@@ -4624,7 +4450,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -4656,7 +4482,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
@@ -4688,7 +4514,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J10" t="s">
         <v>38</v>
@@ -4720,10 +4546,10 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4752,10 +4578,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4784,10 +4610,10 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -4816,10 +4642,10 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -4836,7 +4662,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4867,16 +4693,16 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -4896,19 +4722,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" t="s">
         <v>170</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s">
-        <v>172</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -4928,19 +4754,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4960,19 +4786,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -4992,19 +4818,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -5024,19 +4850,19 @@
         <v>44865.828298611101</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -5056,19 +4882,19 @@
         <v>44873.393229166701</v>
       </c>
       <c r="E7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
         <v>181</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>182</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I7" t="s">
-        <v>184</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -5088,19 +4914,19 @@
         <v>44873.393449074101</v>
       </c>
       <c r="E8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>181</v>
       </c>
-      <c r="F8" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>183</v>
-      </c>
       <c r="I8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -5120,7 +4946,7 @@
         <v>44882.803460648101</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -5132,7 +4958,7 @@
         <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -5152,19 +4978,19 @@
         <v>44971.953680555598</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -5184,19 +5010,19 @@
         <v>44971.953680555598</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -5213,10 +5039,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5242,19 +5068,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" t="s">
         <v>193</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" t="s">
         <v>194</v>
-      </c>
-      <c r="G1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" t="s">
-        <v>196</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -5274,13 +5100,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -5303,13 +5129,13 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
         <v>199</v>
-      </c>
-      <c r="F3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G3" t="s">
-        <v>201</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -5332,10 +5158,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -5358,13 +5184,13 @@
         <v>44942.757025462997</v>
       </c>
       <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" t="s">
         <v>204</v>
-      </c>
-      <c r="F5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G5" t="s">
-        <v>206</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -5387,10 +5213,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -5413,10 +5239,10 @@
         <v>44984.400081018503</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -5439,13 +5265,13 @@
         <v>44887.691469907397</v>
       </c>
       <c r="E8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -5468,13 +5294,13 @@
         <v>44965.452013888898</v>
       </c>
       <c r="E9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -5497,13 +5323,13 @@
         <v>44869.679618055503</v>
       </c>
       <c r="E10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -5526,10 +5352,10 @@
         <v>44873.394305555601</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -5552,10 +5378,10 @@
         <v>44873.394861111097</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -5578,13 +5404,13 @@
         <v>44873.397835648102</v>
       </c>
       <c r="E13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H13" t="s">
         <v>220</v>
-      </c>
-      <c r="F13" t="s">
-        <v>221</v>
-      </c>
-      <c r="H13" t="s">
-        <v>222</v>
       </c>
       <c r="I13">
         <v>6</v>
@@ -5607,13 +5433,13 @@
         <v>44873.404872685198</v>
       </c>
       <c r="E14" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" t="s">
         <v>223</v>
-      </c>
-      <c r="F14" t="s">
-        <v>224</v>
-      </c>
-      <c r="H14" t="s">
-        <v>225</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -5636,13 +5462,13 @@
         <v>44873.948194444398</v>
       </c>
       <c r="E15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" t="s">
         <v>226</v>
-      </c>
-      <c r="F15" t="s">
-        <v>227</v>
-      </c>
-      <c r="G15" t="s">
-        <v>228</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -5665,13 +5491,13 @@
         <v>44873.948611111096</v>
       </c>
       <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" t="s">
         <v>229</v>
-      </c>
-      <c r="F16" t="s">
-        <v>230</v>
-      </c>
-      <c r="G16" t="s">
-        <v>231</v>
       </c>
       <c r="I16">
         <v>6</v>
@@ -5694,13 +5520,13 @@
         <v>44880.940173611103</v>
       </c>
       <c r="E17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" t="s">
+        <v>231</v>
+      </c>
+      <c r="H17" t="s">
         <v>232</v>
-      </c>
-      <c r="F17" t="s">
-        <v>233</v>
-      </c>
-      <c r="H17" t="s">
-        <v>234</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -5723,13 +5549,13 @@
         <v>44880.941412036998</v>
       </c>
       <c r="E18" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" t="s">
         <v>235</v>
-      </c>
-      <c r="F18" t="s">
-        <v>236</v>
-      </c>
-      <c r="H18" t="s">
-        <v>237</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -5743,7 +5569,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>44971.954965277801</v>
@@ -5752,10 +5578,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I19">
         <v>9</v>
@@ -5769,7 +5595,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>44971.955520833297</v>
@@ -5778,10 +5604,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E20" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I20">
         <v>9</v>
@@ -5795,7 +5621,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>44971.956076388902</v>
@@ -5804,10 +5630,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G21" s="2"/>
       <c r="I21">
@@ -5822,7 +5648,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>44983.917581018497</v>
@@ -5831,10 +5657,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I22">
         <v>9</v>
@@ -5848,7 +5674,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>44983.917893518497</v>
@@ -5857,10 +5683,10 @@
         <v>44984.409745370402</v>
       </c>
       <c r="E23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -5874,7 +5700,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>44983.917893518497</v>
@@ -5882,11 +5708,11 @@
       <c r="C24" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>248</v>
+      <c r="E24" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="F24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24">
@@ -5901,7 +5727,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>44983.917893518497</v>
@@ -5909,11 +5735,11 @@
       <c r="C25" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>250</v>
+      <c r="E25" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="F25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G25" s="5"/>
       <c r="I25">
@@ -5928,7 +5754,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>44983.917893518497</v>
@@ -5936,14 +5762,14 @@
       <c r="C26" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F26" t="s">
+        <v>251</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="F26" t="s">
-        <v>253</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -5957,7 +5783,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>44983.917893518497</v>
@@ -5965,11 +5791,11 @@
       <c r="C27" s="1">
         <v>44984.409745370402</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>255</v>
+      <c r="E27" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="F27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G27" s="5">
         <v>25</v>
@@ -5983,6 +5809,38 @@
       <c r="K27">
         <v>0</v>
       </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="E31" s="3"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -5996,7 +5854,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6004,7 +5862,7 @@
     <col min="2" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
@@ -6026,21 +5884,21 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H1" t="s">
         <v>123</v>
       </c>
       <c r="I1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>44984.656585648103</v>
@@ -6052,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -6066,7 +5924,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>44984.6566550926</v>
@@ -6078,7 +5936,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -6093,5 +5951,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
🎈 perf(Optimize menu front-end component field length, and user model class method optimization): 优化菜单前端组件字段长度，以及用户模型类方法优化
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitpush\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EE556-345F-4EC3-84A1-48D5837A808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6316899-CB43-4D9F-BF12-EE05E3C1067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1740" windowWidth="29040" windowHeight="16440" tabRatio="887" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="300">
   <si>
     <t>title</t>
   </si>
@@ -1010,6 +1010,43 @@
   <si>
     <t>ranyong</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>项目</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模块</t>
+    </r>
+  </si>
+  <si>
+    <t>ep:calendar</t>
+  </si>
+  <si>
+    <t>/projectormodule</t>
+  </si>
+  <si>
+    <t>项目列表</t>
+  </si>
+  <si>
+    <t>views/Vadmin/ProjectOrModule/Project</t>
+  </si>
+  <si>
+    <t>project</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1115,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1090,6 +1127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1366,18 +1404,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="19" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="19" max="20" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -3534,6 +3572,118 @@
         <v>45183.466342592597</v>
       </c>
       <c r="V39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B40" t="s">
+        <v>295</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>296</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>81</v>
+      </c>
+      <c r="S40" s="9">
+        <v>45233.746180555558</v>
+      </c>
+      <c r="T40" s="9">
+        <v>45233.747083333335</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D41" t="s">
+        <v>298</v>
+      </c>
+      <c r="E41" t="s">
+        <v>299</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>81</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>82</v>
+      </c>
+      <c r="S41" s="9">
+        <v>45233.748206018521</v>
+      </c>
+      <c r="T41" s="9">
+        <v>45233.748206018521</v>
+      </c>
+      <c r="V41">
         <v>0</v>
       </c>
     </row>
@@ -3551,16 +3701,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="52.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="52.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3598,7 +3748,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2">
         <v>7</v>
       </c>
@@ -3630,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3">
         <v>8</v>
       </c>
@@ -3772,12 +3922,12 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3858,18 +4008,18 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="7" max="7" width="72.28515625" customWidth="1"/>
+    <col min="7" max="7" width="72.33203125" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -3922,7 +4072,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="136.5">
+    <row r="2" spans="1:16" ht="115.8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3984,7 +4134,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4017,14 +4167,14 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4188,13 +4338,13 @@
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4665,15 +4815,15 @@
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -4999,7 +5149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5041,16 +5191,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="67.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="67.88671875" customWidth="1"/>
     <col min="8" max="8" width="98" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5619,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5698,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5725,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5752,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="15">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5781,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="15">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5818,25 +5968,25 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="15">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="3"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" ht="15">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="E31" s="3"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" ht="15">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="E32" s="3"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" ht="15">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="E33" s="3"/>
@@ -5857,14 +6007,14 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5896,7 +6046,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
🎈 perf(Optimize initial data updates ): 优化初始化数据更新
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitpush\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6316899-CB43-4D9F-BF12-EE05E3C1067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A3A3F-5734-4D58-966A-5BA4FDB39571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="312">
   <si>
     <t>title</t>
   </si>
@@ -1019,7 +1019,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>/</t>
     </r>
@@ -1047,6 +1047,42 @@
   </si>
   <si>
     <t>project</t>
+  </si>
+  <si>
+    <t>部门管理</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Auth/Dept/Dept</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>数据权限范围</t>
+  </si>
+  <si>
+    <t>sys_vadmin_data_range</t>
+  </si>
+  <si>
+    <t>仅本人数据权限</t>
+  </si>
+  <si>
+    <t>本部门数据权限</t>
+  </si>
+  <si>
+    <t>本部门及以下数据权限</t>
+  </si>
+  <si>
+    <t>自定义数据权限</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>全部数据权限</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1109,13 +1145,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1128,9 +1165,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{FB2A260C-2442-4543-995F-381788358A55}"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1404,18 +1448,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="19" max="20" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="19" max="20" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -3576,120 +3621,181 @@
       </c>
     </row>
     <row r="40" spans="1:22">
-      <c r="A40" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B40" t="s">
-        <v>295</v>
-      </c>
-      <c r="D40" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" t="s">
-        <v>296</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-      <c r="R40">
+      <c r="A40" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" s="10">
+        <v>2</v>
+      </c>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10">
+        <v>0</v>
+      </c>
+      <c r="M40" s="10">
+        <v>1</v>
+      </c>
+      <c r="N40" s="10">
+        <v>0</v>
+      </c>
+      <c r="O40" s="10">
+        <v>0</v>
+      </c>
+      <c r="P40" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="10">
+        <v>0</v>
+      </c>
+      <c r="R40" s="10">
         <v>81</v>
       </c>
-      <c r="S40" s="9">
-        <v>45233.746180555558</v>
-      </c>
-      <c r="T40" s="9">
-        <v>45233.747083333335</v>
-      </c>
-      <c r="V40">
+      <c r="S40" s="11">
+        <v>45278.950706018521</v>
+      </c>
+      <c r="T40" s="11">
+        <v>45278.950706018521</v>
+      </c>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B41" t="s">
+        <v>295</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>296</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>81</v>
+      </c>
+      <c r="S41" s="9">
+        <v>45233.746180555558</v>
+      </c>
+      <c r="T41" s="9">
+        <v>45233.747083333335</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>298</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>299</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
         <v>81</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>1</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
         <v>82</v>
       </c>
-      <c r="S41" s="9">
+      <c r="S42" s="9">
         <v>45233.748206018521</v>
       </c>
-      <c r="T41" s="9">
+      <c r="T42" s="9">
         <v>45233.748206018521</v>
       </c>
-      <c r="V41">
+      <c r="V42">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3701,16 +3807,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="52.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3748,7 +3854,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>7</v>
       </c>
@@ -3780,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>8</v>
       </c>
@@ -3922,12 +4028,12 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -4008,18 +4114,18 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="7" max="7" width="72.33203125" customWidth="1"/>
+    <col min="7" max="7" width="72.28515625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -4072,7 +4178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="115.8">
+    <row r="2" spans="1:16" ht="136.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4131,10 +4237,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4161,166 +4267,200 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
+      <c r="A1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>44839.919247685182</v>
+      </c>
+      <c r="G2" s="13">
+        <v>44842.58143518518</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13">
+        <v>44842.581620370365</v>
+      </c>
+      <c r="G3" s="13">
+        <v>44842.581620370365</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="13">
+        <v>44898.991770833338</v>
+      </c>
+      <c r="G4" s="13">
+        <v>44898.991770833338</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13">
+        <v>44898.992488425931</v>
+      </c>
+      <c r="G5" s="13">
+        <v>44898.992488425931</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="12">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44839.919247685197</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44842.581435185202</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44842.581620370402</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44842.581620370402</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44898.991770833301</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44898.991770833301</v>
-      </c>
-      <c r="D4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44898.992488425902</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44898.992488425902</v>
-      </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45102.705092592601</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45107.391307870399</v>
-      </c>
-      <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="F6" s="13">
+        <v>45102.705092592594</v>
+      </c>
+      <c r="G6" s="13">
+        <v>45107.39130787037</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13">
+        <v>45281.775648148148</v>
+      </c>
+      <c r="G7" s="13">
+        <v>45281.775648148148</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4332,472 +4472,668 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="K1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14">
+        <v>2</v>
+      </c>
+      <c r="I2" s="15">
+        <v>44841.505358796298</v>
+      </c>
+      <c r="J2" s="15">
+        <v>44841.505578703705</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
+        <v>4</v>
+      </c>
+      <c r="I3" s="15">
+        <v>44842.580231481479</v>
+      </c>
+      <c r="J3" s="15">
+        <v>44842.580231481479</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I4" s="15">
+        <v>44842.586979166663</v>
+      </c>
+      <c r="J4" s="15">
+        <v>44842.587245370371</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14">
+        <v>2</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
+        <v>6</v>
+      </c>
+      <c r="I5" s="15">
+        <v>44842.587083333332</v>
+      </c>
+      <c r="J5" s="15">
+        <v>44842.587083333332</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>2</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" t="s">
-        <v>148</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="I6" s="15">
+        <v>44842.587175925924</v>
+      </c>
+      <c r="J6" s="15">
+        <v>44842.587175925924</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <v>3</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
+        <v>8</v>
+      </c>
+      <c r="I7" s="15">
+        <v>44898.992048611115</v>
+      </c>
+      <c r="J7" s="15">
+        <v>44898.992048611115</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14">
+        <v>3</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
+        <v>9</v>
+      </c>
+      <c r="I8" s="15">
+        <v>44898.992210648154</v>
+      </c>
+      <c r="J8" s="15">
+        <v>44898.992210648154</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <v>4</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14">
+        <v>10</v>
+      </c>
+      <c r="I9" s="15">
+        <v>44898.992638888893</v>
+      </c>
+      <c r="J9" s="15">
+        <v>44898.992638888893</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14">
+        <v>11</v>
+      </c>
+      <c r="I10" s="15">
+        <v>44898.992835648154</v>
+      </c>
+      <c r="J10" s="15">
+        <v>44898.992835648154</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14">
+        <v>3</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14">
+        <v>12</v>
+      </c>
+      <c r="I11" s="15">
+        <v>44980.950659722221</v>
+      </c>
+      <c r="J11" s="15">
+        <v>44980.953773148147</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <v>5</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14">
+        <v>14</v>
+      </c>
+      <c r="I12" s="15">
+        <v>45102.705671296295</v>
+      </c>
+      <c r="J12" s="15">
+        <v>45103.66128472222</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14">
+        <v>15</v>
+      </c>
+      <c r="I13" s="15">
+        <v>45102.706574074073</v>
+      </c>
+      <c r="J13" s="15">
+        <v>45102.706574074073</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14">
+        <v>16</v>
+      </c>
+      <c r="I14" s="15">
+        <v>45102.706724537034</v>
+      </c>
+      <c r="J14" s="15">
+        <v>45103.661400462966</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>6</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14">
+        <v>17</v>
+      </c>
+      <c r="I15" s="15">
+        <v>45281.777569444443</v>
+      </c>
+      <c r="J15" s="15">
+        <v>45257.65048611111</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="14">
+        <v>6</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14">
+        <v>18</v>
+      </c>
+      <c r="I16" s="15">
+        <v>45281.777731481481</v>
+      </c>
+      <c r="J16" s="15">
+        <v>45257.651412037034</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>2</v>
+      </c>
+      <c r="F17" s="14">
+        <v>6</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14">
+        <v>19</v>
+      </c>
+      <c r="I17" s="15">
+        <v>45281.777847222227</v>
+      </c>
+      <c r="J17" s="15">
+        <v>45257.651539351849</v>
+      </c>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <v>3</v>
+      </c>
+      <c r="F18" s="14">
+        <v>6</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="I18" s="15">
+        <v>45281.777951388889</v>
+      </c>
+      <c r="J18" s="15">
+        <v>45257.651597222219</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14">
+        <v>4</v>
+      </c>
+      <c r="F19" s="14">
+        <v>6</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44841.505358796298</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44841.505578703698</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44842.580231481501</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44842.580231481501</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>150</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44842.586979166699</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44842.5872453704</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44842.587083333303</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44842.587083333303</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44842.587175925903</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44842.587175925903</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44898.9920486111</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44898.9920486111</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>154</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44898.992210648197</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44898.992210648197</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44898.9926388889</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44898.9926388889</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>156</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44898.992835648198</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44898.992835648198</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>157</v>
-      </c>
-      <c r="J10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44980.950659722199</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44980.953773148103</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>158</v>
-      </c>
-      <c r="J11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45102.705671296302</v>
-      </c>
-      <c r="C12" s="1">
-        <v>45103.661284722199</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>159</v>
-      </c>
-      <c r="J12" t="s">
-        <v>160</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45102.706574074102</v>
-      </c>
-      <c r="C13" s="1">
-        <v>45102.706574074102</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>161</v>
-      </c>
-      <c r="J13" t="s">
-        <v>162</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45102.706724536998</v>
-      </c>
-      <c r="C14" s="1">
-        <v>45103.661400463003</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14" t="s">
-        <v>163</v>
-      </c>
-      <c r="J14" t="s">
-        <v>164</v>
-      </c>
-      <c r="L14">
+      <c r="I19" s="15">
+        <v>45281.778078703705</v>
+      </c>
+      <c r="J19" s="15">
+        <v>45257.651655092588</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14">
         <v>0</v>
       </c>
     </row>
@@ -4815,15 +5151,15 @@
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5149,7 +5485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5191,16 +5527,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" customWidth="1"/>
-    <col min="7" max="7" width="67.88671875" customWidth="1"/>
+    <col min="2" max="3" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" customWidth="1"/>
     <col min="8" max="8" width="98" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5769,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5848,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5875,7 +6211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5902,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5931,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5968,25 +6304,25 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="15">
+    <row r="30" spans="1:11">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="3"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:11" ht="15">
+    <row r="31" spans="1:11">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="E31" s="3"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="15">
+    <row r="32" spans="1:11">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="E32" s="3"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7" ht="15">
+    <row r="33" spans="2:7">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="E33" s="3"/>
@@ -6007,14 +6343,14 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6046,7 +6382,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
🎈 perf(optimized code): 优化代码
</commit_message>
<xml_diff>
--- a/scripts/initialize/data/init.xlsx
+++ b/scripts/initialize/data/init.xlsx
@@ -8,28 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitpush\Sakura_K\scripts\initialize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A3A3F-5734-4D58-966A-5BA4FDB39571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B914B97-C2CA-4A2C-847B-126197B140C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1305" windowWidth="29040" windowHeight="16440" tabRatio="887" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vadmin_auth_menu" sheetId="1" r:id="rId1"/>
     <sheet name="vadmin_auth_role" sheetId="2" r:id="rId2"/>
     <sheet name="vadmin_auth_user" sheetId="3" r:id="rId3"/>
     <sheet name="vadmin_auth_user_roles" sheetId="9" r:id="rId4"/>
-    <sheet name="vadmin_system_dict_type" sheetId="5" r:id="rId5"/>
-    <sheet name="vadmin_system_dict_details" sheetId="6" r:id="rId6"/>
-    <sheet name="vadmin_system_settings_tab" sheetId="8" r:id="rId7"/>
-    <sheet name="vadmin_system_settings" sheetId="7" r:id="rId8"/>
-    <sheet name="vadmin_help_issue_category" sheetId="10" r:id="rId9"/>
-    <sheet name="vadmin_help_issue" sheetId="11" r:id="rId10"/>
+    <sheet name="vadmin_auth_dept" sheetId="12" r:id="rId5"/>
+    <sheet name="vadmin_auth_user_depts" sheetId="13" r:id="rId6"/>
+    <sheet name="vadmin_system_dict_type" sheetId="5" r:id="rId7"/>
+    <sheet name="vadmin_system_dict_details" sheetId="6" r:id="rId8"/>
+    <sheet name="vadmin_system_settings_tab" sheetId="8" r:id="rId9"/>
+    <sheet name="vadmin_system_settings" sheetId="7" r:id="rId10"/>
+    <sheet name="vadmin_help_issue_category" sheetId="10" r:id="rId11"/>
+    <sheet name="vadmin_help_issue" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="316">
   <si>
     <t>title</t>
   </si>
@@ -1012,16 +1014,59 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>部门管理</t>
+  </si>
+  <si>
+    <t>views/Vadmin/Auth/Dept/Dept</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>数据权限范围</t>
+  </si>
+  <si>
+    <t>sys_vadmin_data_range</t>
+  </si>
+  <si>
+    <t>仅本人数据权限</t>
+  </si>
+  <si>
+    <t>本部门数据权限</t>
+  </si>
+  <si>
+    <t>本部门及以下数据权限</t>
+  </si>
+  <si>
+    <t>自定义数据权限</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>全部数据权限</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>dept_key</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>total_group</t>
+  </si>
+  <si>
     <r>
-      <t>项目</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
+      <t xml:space="preserve">Sakura_K </t>
     </r>
     <r>
       <rPr>
@@ -1030,59 +1075,23 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>模块</t>
+      <t>开发团队</t>
     </r>
-  </si>
-  <si>
-    <t>ep:calendar</t>
-  </si>
-  <si>
-    <t>/projectormodule</t>
-  </si>
-  <si>
-    <t>项目列表</t>
-  </si>
-  <si>
-    <t>views/Vadmin/ProjectOrModule/Project</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>部门管理</t>
-  </si>
-  <si>
-    <t>views/Vadmin/Auth/Dept/Dept</t>
-  </si>
-  <si>
-    <t>dept</t>
-  </si>
-  <si>
-    <t>数据权限范围</t>
-  </si>
-  <si>
-    <t>sys_vadmin_data_range</t>
-  </si>
-  <si>
-    <t>仅本人数据权限</t>
-  </si>
-  <si>
-    <t>本部门数据权限</t>
-  </si>
-  <si>
-    <t>本部门及以下数据权限</t>
-  </si>
-  <si>
-    <t>自定义数据权限</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>全部数据权限</t>
-  </si>
-  <si>
-    <t>4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ranyong1209@gmail.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>dept_id</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1161,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1164,11 +1173,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
@@ -1448,10 +1452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3621,174 +3625,62 @@
       </c>
     </row>
     <row r="40" spans="1:22">
-      <c r="A40" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F40" s="10">
-        <v>0</v>
-      </c>
-      <c r="G40" s="10">
-        <v>0</v>
-      </c>
-      <c r="H40" s="10">
-        <v>0</v>
-      </c>
-      <c r="I40" s="10" t="s">
+      <c r="A40" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F40" s="9">
+        <v>0</v>
+      </c>
+      <c r="G40" s="9">
+        <v>0</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="9">
         <v>2</v>
       </c>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10">
-        <v>0</v>
-      </c>
-      <c r="M40" s="10">
-        <v>1</v>
-      </c>
-      <c r="N40" s="10">
-        <v>0</v>
-      </c>
-      <c r="O40" s="10">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="10">
-        <v>0</v>
-      </c>
-      <c r="R40" s="10">
+      <c r="K40" s="9"/>
+      <c r="L40" s="9">
+        <v>0</v>
+      </c>
+      <c r="M40" s="9">
+        <v>1</v>
+      </c>
+      <c r="N40" s="9">
+        <v>0</v>
+      </c>
+      <c r="O40" s="9">
+        <v>0</v>
+      </c>
+      <c r="P40" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="9">
+        <v>0</v>
+      </c>
+      <c r="R40" s="9">
         <v>81</v>
       </c>
-      <c r="S40" s="11">
+      <c r="S40" s="10">
         <v>45278.950706018521</v>
       </c>
-      <c r="T40" s="11">
+      <c r="T40" s="10">
         <v>45278.950706018521</v>
       </c>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="A41" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B41" t="s">
-        <v>295</v>
-      </c>
-      <c r="D41" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" t="s">
-        <v>296</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>1</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-      <c r="R41">
-        <v>81</v>
-      </c>
-      <c r="S41" s="9">
-        <v>45233.746180555558</v>
-      </c>
-      <c r="T41" s="9">
-        <v>45233.747083333335</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
-      <c r="A42" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="D42" t="s">
-        <v>298</v>
-      </c>
-      <c r="E42" t="s">
-        <v>299</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>81</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>1</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42">
-        <v>0</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>82</v>
-      </c>
-      <c r="S42" s="9">
-        <v>45233.748206018521</v>
-      </c>
-      <c r="T42" s="9">
-        <v>45233.748206018521</v>
-      </c>
-      <c r="V42">
+      <c r="U40" s="9"/>
+      <c r="V40" s="9">
         <v>0</v>
       </c>
     </row>
@@ -3800,6 +3692,924 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" customWidth="1"/>
+    <col min="8" max="8" width="98" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44984.400081018503</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44984.400081018503</v>
+      </c>
+      <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44984.400081018503</v>
+      </c>
+      <c r="E4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44942.757025462997</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44984.400081018503</v>
+      </c>
+      <c r="E6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44865.8664699074</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44984.400081018503</v>
+      </c>
+      <c r="E7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44865.868032407401</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44887.691469907397</v>
+      </c>
+      <c r="E8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44869.576631944401</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44965.452013888898</v>
+      </c>
+      <c r="E9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>212</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44869.577037037001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44869.679618055503</v>
+      </c>
+      <c r="E10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44873.394305555601</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44873.394305555601</v>
+      </c>
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" t="s">
+        <v>215</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44873.394861111097</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44873.394861111097</v>
+      </c>
+      <c r="E12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44873.397835648102</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44873.397835648102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44873.404872685198</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44873.404872685198</v>
+      </c>
+      <c r="E14" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44873.948194444398</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44873.948194444398</v>
+      </c>
+      <c r="E15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" t="s">
+        <v>226</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44873.948611111096</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44873.948611111096</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" t="s">
+        <v>229</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44880.940173611103</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44880.940173611103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" t="s">
+        <v>231</v>
+      </c>
+      <c r="H17" t="s">
+        <v>232</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44880.941412036998</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44880.941412036998</v>
+      </c>
+      <c r="E18" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" t="s">
+        <v>235</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44971.954965277801</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E19" t="s">
+        <v>236</v>
+      </c>
+      <c r="F19" t="s">
+        <v>237</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44971.955520833297</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44971.956076388902</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F21" t="s">
+        <v>241</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44983.917581018497</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F22" t="s">
+        <v>243</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44983.917893518497</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>245</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44983.917893518497</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F24" t="s">
+        <v>247</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44983.917893518497</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F25" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44983.917893518497</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F26" t="s">
+        <v>251</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44983.917893518497</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44984.409745370402</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F27" t="s">
+        <v>254</v>
+      </c>
+      <c r="G27" s="5">
+        <v>25</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="E31" s="3"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44984.656585648103</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44984.656585648103</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44984.6566550926</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44984.6566550926</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -4108,10 +4918,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4119,16 +4929,17 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="7" max="7" width="72.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4141,44 +4952,47 @@
       <c r="D1" t="s">
         <v>118</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>122</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>123</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>124</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>125</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>126</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="136.5">
+    <row r="2" spans="1:17" ht="136.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4191,44 +5005,51 @@
       <c r="D2">
         <v>13206269804</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="O2">
-        <v>0</v>
+      <c r="N2" s="1">
+        <v>45197.896111111113</v>
       </c>
       <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{F8AEA984-9637-4FAE-8645-FAC22C399F20}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{F8AEA984-9637-4FAE-8645-FAC22C399F20}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{96969C4C-CBFB-42EE-A2EA-C73AE442EECB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4266,6 +5087,130 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7413C65F-4B34-4079-A0BF-0AB53C509D6C}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45278.952164351846</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45281.748402777775</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3AAD62-24FE-4485-800A-9DBD4FE8B326}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -4284,183 +5229,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="12">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12">
-        <v>1</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
         <v>44839.919247685182</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="10">
         <v>44842.58143518518</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12">
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>44842.581620370365</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="10">
         <v>44842.581620370365</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="12">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12">
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9">
         <v>3</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>44898.991770833338</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="10">
         <v>44898.991770833338</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="12">
-        <v>0</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12">
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>44898.992488425931</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="10">
         <v>44898.992488425931</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="12">
-        <v>0</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>5</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>45102.705092592594</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="10">
         <v>45107.39130787037</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12">
+      <c r="A7" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <v>6</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>45281.775648148148</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="10">
         <v>45281.775648148148</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4470,7 +5415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -4488,652 +5433,652 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="14">
-        <v>0</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14">
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9">
         <v>2</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="10">
         <v>44841.505358796298</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="10">
         <v>44841.505578703705</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="14">
-        <v>0</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14">
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9">
         <v>4</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="10">
         <v>44842.580231481479</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="10">
         <v>44842.580231481479</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="14">
-        <v>0</v>
-      </c>
-      <c r="D4" s="14">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
         <v>5</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="10">
         <v>44842.586979166663</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="10">
         <v>44842.587245370371</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1</v>
-      </c>
-      <c r="F5" s="14">
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
         <v>2</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <v>6</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="10">
         <v>44842.587083333332</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="10">
         <v>44842.587083333332</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="14">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <v>7</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="10">
         <v>44842.587175925924</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="10">
         <v>44842.587175925924</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14">
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
         <v>3</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <v>8</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="10">
         <v>44898.992048611115</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="10">
         <v>44898.992048611115</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
         <v>3</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>9</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="10">
         <v>44898.992210648154</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="10">
         <v>44898.992210648154</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
         <v>4</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
         <v>10</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="10">
         <v>44898.992638888893</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="10">
         <v>44898.992638888893</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
         <v>4</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>11</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="10">
         <v>44898.992835648154</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="10">
         <v>44898.992835648154</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
         <v>2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <v>12</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="10">
         <v>44980.950659722221</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="10">
         <v>44980.953773148147</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
         <v>5</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
         <v>14</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="10">
         <v>45102.705671296295</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="10">
         <v>45103.66128472222</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="14">
-        <v>0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14">
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
         <v>5</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
         <v>15</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="10">
         <v>45102.706574074073</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="10">
         <v>45102.706574074073</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
         <v>2</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="9">
         <v>5</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <v>16</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="10">
         <v>45102.706724537034</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="10">
         <v>45103.661400462966</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>6</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <v>17</v>
+      </c>
+      <c r="I15" s="10">
+        <v>45281.777569444443</v>
+      </c>
+      <c r="J15" s="10">
+        <v>45257.65048611111</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>6</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
+        <v>18</v>
+      </c>
+      <c r="I16" s="10">
+        <v>45281.777731481481</v>
+      </c>
+      <c r="J16" s="10">
+        <v>45257.651412037034</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="9">
+        <v>6</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9">
+        <v>19</v>
+      </c>
+      <c r="I17" s="10">
+        <v>45281.777847222227</v>
+      </c>
+      <c r="J17" s="10">
+        <v>45257.651539351849</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>3</v>
+      </c>
+      <c r="F18" s="9">
+        <v>6</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9">
+        <v>20</v>
+      </c>
+      <c r="I18" s="10">
+        <v>45281.777951388889</v>
+      </c>
+      <c r="J18" s="10">
+        <v>45257.651597222219</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>4</v>
+      </c>
+      <c r="F19" s="9">
         <v>6</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14">
-        <v>17</v>
-      </c>
-      <c r="I15" s="15">
-        <v>45281.777569444443</v>
-      </c>
-      <c r="J15" s="15">
-        <v>45257.65048611111</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="D16" s="14">
-        <v>0</v>
-      </c>
-      <c r="E16" s="14">
-        <v>1</v>
-      </c>
-      <c r="F16" s="14">
-        <v>6</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14">
-        <v>18</v>
-      </c>
-      <c r="I16" s="15">
-        <v>45281.777731481481</v>
-      </c>
-      <c r="J16" s="15">
-        <v>45257.651412037034</v>
-      </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>2</v>
-      </c>
-      <c r="F17" s="14">
-        <v>6</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14">
-        <v>19</v>
-      </c>
-      <c r="I17" s="15">
-        <v>45281.777847222227</v>
-      </c>
-      <c r="J17" s="15">
-        <v>45257.651539351849</v>
-      </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="C18" s="14">
-        <v>0</v>
-      </c>
-      <c r="D18" s="14">
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
-        <v>3</v>
-      </c>
-      <c r="F18" s="14">
-        <v>6</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14">
-        <v>20</v>
-      </c>
-      <c r="I18" s="15">
-        <v>45281.777951388889</v>
-      </c>
-      <c r="J18" s="15">
-        <v>45257.651597222219</v>
-      </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14">
-        <v>0</v>
-      </c>
-      <c r="E19" s="14">
-        <v>4</v>
-      </c>
-      <c r="F19" s="14">
-        <v>6</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9">
         <v>21</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="10">
         <v>45281.778078703705</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="10">
         <v>45257.651655092588</v>
       </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9">
         <v>0</v>
       </c>
     </row>
@@ -5143,7 +6088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -5521,922 +6466,4 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="3" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="67.85546875" customWidth="1"/>
-    <col min="8" max="8" width="98" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44984.400081018503</v>
-      </c>
-      <c r="E2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44984.400081018503</v>
-      </c>
-      <c r="E3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" t="s">
-        <v>198</v>
-      </c>
-      <c r="G3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44984.400081018503</v>
-      </c>
-      <c r="E4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" t="s">
-        <v>201</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44942.757025462997</v>
-      </c>
-      <c r="E5" t="s">
-        <v>202</v>
-      </c>
-      <c r="F5" t="s">
-        <v>203</v>
-      </c>
-      <c r="G5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44984.400081018503</v>
-      </c>
-      <c r="E6" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" t="s">
-        <v>206</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44865.8664699074</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44984.400081018503</v>
-      </c>
-      <c r="E7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F7" t="s">
-        <v>208</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44865.868032407401</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44887.691469907397</v>
-      </c>
-      <c r="E8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44869.576631944401</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44965.452013888898</v>
-      </c>
-      <c r="E9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F9" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9" t="s">
-        <v>212</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44869.577037037001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44869.679618055503</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" t="s">
-        <v>178</v>
-      </c>
-      <c r="G10" t="s">
-        <v>213</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44873.394305555601</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44873.394305555601</v>
-      </c>
-      <c r="E11" t="s">
-        <v>214</v>
-      </c>
-      <c r="F11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44873.394861111097</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44873.394861111097</v>
-      </c>
-      <c r="E12" t="s">
-        <v>216</v>
-      </c>
-      <c r="F12" t="s">
-        <v>217</v>
-      </c>
-      <c r="I12">
-        <v>6</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44873.397835648102</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44873.397835648102</v>
-      </c>
-      <c r="E13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H13" t="s">
-        <v>220</v>
-      </c>
-      <c r="I13">
-        <v>6</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44873.404872685198</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44873.404872685198</v>
-      </c>
-      <c r="E14" t="s">
-        <v>221</v>
-      </c>
-      <c r="F14" t="s">
-        <v>222</v>
-      </c>
-      <c r="H14" t="s">
-        <v>223</v>
-      </c>
-      <c r="I14">
-        <v>6</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44873.948194444398</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44873.948194444398</v>
-      </c>
-      <c r="E15" t="s">
-        <v>224</v>
-      </c>
-      <c r="F15" t="s">
-        <v>225</v>
-      </c>
-      <c r="G15" t="s">
-        <v>226</v>
-      </c>
-      <c r="I15">
-        <v>6</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44873.948611111096</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44873.948611111096</v>
-      </c>
-      <c r="E16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F16" t="s">
-        <v>228</v>
-      </c>
-      <c r="G16" t="s">
-        <v>229</v>
-      </c>
-      <c r="I16">
-        <v>6</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44880.940173611103</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44880.940173611103</v>
-      </c>
-      <c r="E17" t="s">
-        <v>230</v>
-      </c>
-      <c r="F17" t="s">
-        <v>231</v>
-      </c>
-      <c r="H17" t="s">
-        <v>232</v>
-      </c>
-      <c r="I17">
-        <v>6</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44880.941412036998</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44880.941412036998</v>
-      </c>
-      <c r="E18" t="s">
-        <v>233</v>
-      </c>
-      <c r="F18" t="s">
-        <v>234</v>
-      </c>
-      <c r="H18" t="s">
-        <v>235</v>
-      </c>
-      <c r="I18">
-        <v>6</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44971.954965277801</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E19" t="s">
-        <v>236</v>
-      </c>
-      <c r="F19" t="s">
-        <v>237</v>
-      </c>
-      <c r="I19">
-        <v>9</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>44971.955520833297</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E20" t="s">
-        <v>238</v>
-      </c>
-      <c r="F20" t="s">
-        <v>239</v>
-      </c>
-      <c r="I20">
-        <v>9</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>44971.956076388902</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E21" t="s">
-        <v>240</v>
-      </c>
-      <c r="F21" t="s">
-        <v>241</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="I21">
-        <v>9</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>44983.917581018497</v>
-      </c>
-      <c r="C22" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E22" t="s">
-        <v>242</v>
-      </c>
-      <c r="F22" t="s">
-        <v>243</v>
-      </c>
-      <c r="I22">
-        <v>9</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>44983.917893518497</v>
-      </c>
-      <c r="C23" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E23" t="s">
-        <v>244</v>
-      </c>
-      <c r="F23" t="s">
-        <v>245</v>
-      </c>
-      <c r="I23">
-        <v>9</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>44983.917893518497</v>
-      </c>
-      <c r="C24" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="F24" t="s">
-        <v>247</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="I24">
-        <v>10</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>44983.917893518497</v>
-      </c>
-      <c r="C25" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="F25" t="s">
-        <v>249</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="I25">
-        <v>10</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>44983.917893518497</v>
-      </c>
-      <c r="C26" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F26" t="s">
-        <v>251</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="I26">
-        <v>10</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>44983.917893518497</v>
-      </c>
-      <c r="C27" s="1">
-        <v>44984.409745370402</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="F27" t="s">
-        <v>254</v>
-      </c>
-      <c r="G27" s="5">
-        <v>25</v>
-      </c>
-      <c r="I27">
-        <v>10</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="E30" s="3"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="E31" s="3"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="E32" s="3"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="E33" s="3"/>
-      <c r="G33" s="5"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" t="s">
-        <v>255</v>
-      </c>
-      <c r="H1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44984.656585648103</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44984.656585648103</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44984.6566550926</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44984.6566550926</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>